<commit_message>
Rework RTD a bit
</commit_message>
<xml_diff>
--- a/Examples/Udf/Samples/FunctionTests.xlsx
+++ b/Examples/Udf/Samples/FunctionTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ExcelMVC\Examples\Udf\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2939CD95-C029-4AB4-86DC-706200AF05DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D997424-1071-47E5-AFE1-FD1B631A982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="3472" windowWidth="16552" windowHeight="9871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7410" yWindow="5648" windowWidth="16553" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>uDouble</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>uDateTimeMatrix</t>
+  </si>
+  <si>
+    <t>uAsync</t>
+  </si>
+  <si>
+    <t>uRtdTimer</t>
   </si>
 </sst>
 </file>
@@ -156,6 +162,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="excelmvc.7a9485be72c9497dbdc679a010f036de">
+      <tp t="s">
+        <v>2024-04-11T16:53:56.0357919+10:00Test</v>
+        <stp/>
+        <stp>Test</stp>
+        <tr r="B21" s="1"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -460,7 +481,7 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_xll.uDateTime(NOW())</f>
-        <v>45392.708007986112</v>
+        <v>45393.704120717593</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -627,6 +648,24 @@
       </c>
       <c r="C19" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" cm="1">
+        <f t="array" ref="B20">_xll.uAsync(3,4)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="str" cm="1">
+        <f t="array" ref="B21">_xll.uTimer("Test")</f>
+        <v>Test</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Object array marshal
</commit_message>
<xml_diff>
--- a/Examples/Udf/Samples/FunctionTests.xlsx
+++ b/Examples/Udf/Samples/FunctionTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ExcelMVC\Examples\Udf\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D997424-1071-47E5-AFE1-FD1B631A982E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89D8E73-DEBC-46CB-BA54-617491A51140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="5648" windowWidth="16553" windowHeight="9870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="5663" windowWidth="18555" windowHeight="6645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
     <t>uAsync</t>
   </si>
   <si>
-    <t>uRtdTimer</t>
+    <t>uTimer(RTD)</t>
   </si>
 </sst>
 </file>
@@ -167,9 +167,9 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="excelmvc.7a9485be72c9497dbdc679a010f036de">
+    <main first="excelmvc.830f2665c702478682192b0fb74a7db6">
       <tp t="s">
-        <v>2024-04-11T16:53:56.0357919+10:00Test</v>
+        <v>time:2024-04-13T16:37:50.0544211+10:00 topic:Test</v>
         <stp/>
         <stp>Test</stp>
         <tr r="B21" s="1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_xll.uDateTime(NOW())</f>
-        <v>45393.704120717593</v>
+        <v>45395.693105555554</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -665,7 +665,7 @@
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">_xll.uTimer("Test")</f>
-        <v>Test</v>
+        <v>time:2024-04-13T16:37:50.0544211+10:00 topic:Test</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Int32Array & Int32Matrix
</commit_message>
<xml_diff>
--- a/Examples/Udf/Samples/FunctionTests.xlsx
+++ b/Examples/Udf/Samples/FunctionTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ExcelMVC\Examples\Udf\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D16C50-6AA9-4A6F-8EA7-CB6610DA1A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1788D-24EB-4A81-9B2C-4772763D9F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2483" yWindow="3915" windowWidth="18555" windowHeight="8993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>uDouble</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>uObject(Empty)</t>
+  </si>
+  <si>
+    <t>uInt32Array</t>
+  </si>
+  <si>
+    <t>uInt32Matrix</t>
   </si>
 </sst>
 </file>
@@ -176,9 +182,9 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="excelmvc.524598b742c24963b18c8bf0fd4b51e0">
+    <main first="excelmvc.0c8dda118fe94b09b0ebeece0633f5a4">
       <tp t="s">
-        <v>time:2024-04-13T17:50:53.4999072+10:00 topic:Test</v>
+        <v>time:2024-04-21T09:26:01.6207099+10:00 topic:Test</v>
         <stp/>
         <stp>Test</stp>
         <tr r="B21" s="1"/>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -490,7 +496,7 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_xll.uDateTime(NOW())</f>
-        <v>45395.743679861109</v>
+        <v>45403.393077199071</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -674,7 +680,7 @@
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">_xll.uTimer("Test")</f>
-        <v>time:2024-04-13T17:50:53.4999072+10:00 topic:Test</v>
+        <v>time:2024-04-21T09:26:01.6207099+10:00 topic:Test</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -738,6 +744,60 @@
         <v>0</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" cm="1">
+        <f t="array" ref="B34:E34">_xll.uInt32Array(B35:C36)</f>
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" cm="1">
+        <f t="array" ref="B37:C38">_xll.uInt32Matrix(B35:C36)</f>
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added StringArray & StringMatrix
</commit_message>
<xml_diff>
--- a/Examples/Udf/Samples/FunctionTests.xlsx
+++ b/Examples/Udf/Samples/FunctionTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ExcelMVC\Examples\Udf\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1788D-24EB-4A81-9B2C-4772763D9F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120AEDCE-8F60-46A1-AFE6-1825A81CF83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="2400" windowWidth="13883" windowHeight="10027" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>uDouble</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>uInt32Matrix</t>
+  </si>
+  <si>
+    <t>uStringArray</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -159,9 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,9 +194,9 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="excelmvc.0c8dda118fe94b09b0ebeece0633f5a4">
+    <main first="excelmvc.4c1013d96a124562b0da4c462ee0d61a">
       <tp t="s">
-        <v>time:2024-04-21T09:26:01.6207099+10:00 topic:Test</v>
+        <v>time:2024-04-21T09:43:47.4549880+10:00 topic:Test</v>
         <stp/>
         <stp>Test</stp>
         <tr r="B21" s="1"/>
@@ -457,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -496,7 +508,7 @@
       </c>
       <c r="B3" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_xll.uDateTime(NOW())</f>
-        <v>45403.393077199071</v>
+        <v>45403.405421759257</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -680,7 +692,7 @@
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">_xll.uTimer("Test")</f>
-        <v>time:2024-04-21T09:26:01.6207099+10:00 topic:Test</v>
+        <v>time:2024-04-21T09:43:47.4549880+10:00 topic:Test</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -798,6 +810,57 @@
         <v>4</v>
       </c>
     </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="str" cm="1">
+        <f t="array" ref="B40:E40">_xll.uStringArray(B41:C42)</f>
+        <v>1</v>
+      </c>
+      <c r="C40" t="str">
+        <v>a</v>
+      </c>
+      <c r="D40" t="str">
+        <v>b</v>
+      </c>
+      <c r="E40" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B43" t="str" cm="1">
+        <f t="array" ref="B43:C44">_xll.uStringMatrix(B41:C42)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" t="str">
+        <v>a</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B44" t="str">
+        <v>b</v>
+      </c>
+      <c r="C44" t="str">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>